<commit_message>
Build site at 2022-09-26 16:07:08 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/8800006.xlsx
+++ b/assets/disciplinas/8800006.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Ementa atual:</t>
   </si>
@@ -67,9 +67,7 @@
     <t>Objetivos:</t>
   </si>
   <si>
-    <t>Desenvolver um projeto sobre tema de Engenharia de Produção, similar a situações que os alunos irão encontrar na vida real no efetivo exercício de sua profissão, 
-Aplicar e integrar conhecimentos adquiridos em demais disciplinas de seu curso
-Desenvolver competências técnicas, as relacionadas ao projeto em si, bem como competências transversais (habilidades e atitudes), num ambiente de aprendizagem baseado em PBL (Project-Baed Learning).</t>
+    <t>5840560 - Marco Antonio Carvalho Pereira</t>
   </si>
   <si>
     <t>Objectives:</t>
@@ -78,13 +76,10 @@
     <t>Docentes responsáveis:</t>
   </si>
   <si>
-    <t>5840560 - Marco Antonio Carvalho Pereira</t>
-  </si>
-  <si>
     <t>Programa resumido:</t>
   </si>
   <si>
-    <t>Tópicos que abordem o tema do projeto de seu planejamento a execução.</t>
+    <t>Semestral</t>
   </si>
   <si>
     <t>Short syllabus:</t>
@@ -93,17 +88,6 @@
     <t>Programa:</t>
   </si>
   <si>
-    <t>Noções de Gestão de Projetos
-Organização do tempo: dimensão pessoal;
-Técnicas para a realização de apresentações;
-Noções de Aprendizagem Baseada em Projetos
-Trabalho em Grupo, Equipes e times. 
-Postura e Ética Profissional
-Técnicas para redação de relatório técnico;
-Tutoria de projetos.
-Assuntos Técnicos específicos relacionados com o tema do projeto.</t>
-  </si>
-  <si>
     <t>Syllabus:</t>
   </si>
   <si>
@@ -111,6 +95,9 @@
   </si>
   <si>
     <t>Método:</t>
+  </si>
+  <si>
+    <t>Critério:</t>
   </si>
   <si>
     <t>O método utilizado tem por fundamento a Aprendizagem Baseada em Projetos (PBL) que visa desenvolver as competências técnicas relativas ao tema do projeto, bem como competências transversais, tais como: aprender a aprender, trabalho em equipe, relacionamento interpessoal, aspectos de liderança e capacidade de comunicação, dentre outras.
@@ -119,24 +106,17 @@
 As aulas ocorrerão: 1) através de uma reunião da equipe de trabalho para tratar do projeto, e  2) palestras e dinâmicas relativas ao tema do projeto, conduzidas por professores  ou profissionais de empresas.</t>
   </si>
   <si>
-    <t>Critério:</t>
+    <t>Norma de recuperação:</t>
   </si>
   <si>
     <t>A nota será individual e será a média ponderada de componentes do projeto, tais como: Projeto Preliminar, Projeto Final, envolvimento do aluno com o projeto, Avaliação dos Pares, Apresentação de Trabalhos, dentre outros.
 O detalhamento dos pesos para ponderação da média da disciplina será definido por uma equipe de professores que atuarão na coordenação da disciplina.</t>
   </si>
   <si>
-    <t>Norma de recuperação:</t>
+    <t>Bibliografia:</t>
   </si>
   <si>
     <t>Não há recuperação</t>
-  </si>
-  <si>
-    <t>Bibliografia:</t>
-  </si>
-  <si>
-    <t>Artigos sobre metodologias ativas de aprendizagem e  Project Based Learning.
-Livros e Artigos científicos relacionados com o tema do projeto.</t>
   </si>
 </sst>
 </file>
@@ -492,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -617,93 +597,85 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" ht="60" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="60" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="60" customHeight="1">
+    </row>
+    <row r="15" spans="1:3" ht="120" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="120" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="120" customHeight="1">
-      <c r="A17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="60" customHeight="1">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>27</v>
+      <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" customHeight="1">
       <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="60" customHeight="1">
       <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="120" customHeight="1">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="60" customHeight="1">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C21" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="120" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build site at 2023-04-12 14:53:07 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/8800006.xlsx
+++ b/assets/disciplinas/8800006.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Ementa atual:</t>
   </si>
@@ -67,19 +67,24 @@
     <t>Objetivos:</t>
   </si>
   <si>
+    <t>Desenvolver um projeto sobre tema de Engenharia de Produção, similar a situações que os alunos irão encontrar na vida real no efetivo exercício de sua profissão, 
+Aplicar e integrar conhecimentos adquiridos em demais disciplinas de seu curso
+Desenvolver competências técnicas, as relacionadas ao projeto em si, bem como competências transversais (habilidades e atitudes), num ambiente de aprendizagem baseado em PBL (Project-Baed Learning).</t>
+  </si>
+  <si>
+    <t>Objectives:</t>
+  </si>
+  <si>
+    <t>Docentes responsáveis:</t>
+  </si>
+  <si>
     <t>5840560 - Marco Antonio Carvalho Pereira</t>
   </si>
   <si>
-    <t>Objectives:</t>
-  </si>
-  <si>
-    <t>Docentes responsáveis:</t>
-  </si>
-  <si>
     <t>Programa resumido:</t>
   </si>
   <si>
-    <t>Semestral</t>
+    <t>Tópicos que abordem o tema do projeto de seu planejamento a execução.</t>
   </si>
   <si>
     <t>Short syllabus:</t>
@@ -88,6 +93,17 @@
     <t>Programa:</t>
   </si>
   <si>
+    <t>Noções de Gestão de Projetos
+Organização do tempo: dimensão pessoal;
+Técnicas para a realização de apresentações;
+Noções de Aprendizagem Baseada em Projetos
+Trabalho em Grupo, Equipes e times. 
+Postura e Ética Profissional
+Técnicas para redação de relatório técnico;
+Tutoria de projetos.
+Assuntos Técnicos específicos relacionados com o tema do projeto.</t>
+  </si>
+  <si>
     <t>Syllabus:</t>
   </si>
   <si>
@@ -95,9 +111,6 @@
   </si>
   <si>
     <t>Método:</t>
-  </si>
-  <si>
-    <t>Critério:</t>
   </si>
   <si>
     <t>O método utilizado tem por fundamento a Aprendizagem Baseada em Projetos (PBL) que visa desenvolver as competências técnicas relativas ao tema do projeto, bem como competências transversais, tais como: aprender a aprender, trabalho em equipe, relacionamento interpessoal, aspectos de liderança e capacidade de comunicação, dentre outras.
@@ -106,17 +119,24 @@
 As aulas ocorrerão: 1) através de uma reunião da equipe de trabalho para tratar do projeto, e  2) palestras e dinâmicas relativas ao tema do projeto, conduzidas por professores  ou profissionais de empresas.</t>
   </si>
   <si>
-    <t>Norma de recuperação:</t>
+    <t>Critério:</t>
   </si>
   <si>
     <t>A nota será individual e será a média ponderada de componentes do projeto, tais como: Projeto Preliminar, Projeto Final, envolvimento do aluno com o projeto, Avaliação dos Pares, Apresentação de Trabalhos, dentre outros.
 O detalhamento dos pesos para ponderação da média da disciplina será definido por uma equipe de professores que atuarão na coordenação da disciplina.</t>
   </si>
   <si>
+    <t>Norma de recuperação:</t>
+  </si>
+  <si>
+    <t>Não há recuperação</t>
+  </si>
+  <si>
     <t>Bibliografia:</t>
   </si>
   <si>
-    <t>Não há recuperação</t>
+    <t>Artigos sobre metodologias ativas de aprendizagem e  Project Based Learning.
+Livros e Artigos científicos relacionados com o tema do projeto.</t>
   </si>
 </sst>
 </file>
@@ -472,13 +492,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="30.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="60.7109375" style="3" customWidth="1"/>
   </cols>
@@ -597,85 +617,93 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="60" customHeight="1">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:3">
+      <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="60" customHeight="1">
       <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="120" customHeight="1">
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="120" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="120" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="60" customHeight="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="60" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="120" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="60" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="120" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>